<commit_message>
commit lokasi_ujian, ruang_ujian, and pengawas
</commit_message>
<xml_diff>
--- a/Data SIRIMA Mod B16.xlsx
+++ b/Data SIRIMA Mod B16.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Basdat\TK.exe\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="4635" firstSheet="15" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="JENJANG" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="486" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="657" uniqueCount="329">
   <si>
     <t>nama_fakultas</t>
   </si>
@@ -523,9 +523,6 @@
     <t>tempat</t>
   </si>
   <si>
-    <t>Kampus ABC</t>
-  </si>
-  <si>
     <t>Depok</t>
   </si>
   <si>
@@ -812,6 +809,225 @@
   </si>
   <si>
     <t>13/5/2009 17:00</t>
+  </si>
+  <si>
+    <t>Tangerang</t>
+  </si>
+  <si>
+    <t>Jakarta</t>
+  </si>
+  <si>
+    <t>Universitas Indonesia</t>
+  </si>
+  <si>
+    <t>Prasetya Mulya</t>
+  </si>
+  <si>
+    <t>Universitas Gunadarma</t>
+  </si>
+  <si>
+    <t>Bina Sarana Informatika</t>
+  </si>
+  <si>
+    <t>'22/7/2007 07:00'</t>
+  </si>
+  <si>
+    <t>'22/5/2008 07:00'</t>
+  </si>
+  <si>
+    <t>'21/4/2009 07:00'</t>
+  </si>
+  <si>
+    <t>Universitas Trisakti</t>
+  </si>
+  <si>
+    <t>Universitas Swiss dan Jerman</t>
+  </si>
+  <si>
+    <t>'22/7/2008 07:00'</t>
+  </si>
+  <si>
+    <t>'22/7/2009 07:00'</t>
+  </si>
+  <si>
+    <t>Universitas Negeri Jakarta</t>
+  </si>
+  <si>
+    <t>Universitas Bina Nusantara</t>
+  </si>
+  <si>
+    <t>'22/5/2007 07:00'</t>
+  </si>
+  <si>
+    <t>'22/5/2009 07:00'</t>
+  </si>
+  <si>
+    <t>Universitas Pelita Harapan</t>
+  </si>
+  <si>
+    <t>'21/4/2007 07:00'</t>
+  </si>
+  <si>
+    <t>'21/4/2008 07:00'</t>
+  </si>
+  <si>
+    <t>RUANG_UJIAN</t>
+  </si>
+  <si>
+    <t>7334324392748327</t>
+  </si>
+  <si>
+    <t>Jaron Wahyudi</t>
+  </si>
+  <si>
+    <t>085710283323</t>
+  </si>
+  <si>
+    <t>2843792911203407</t>
+  </si>
+  <si>
+    <t>Gani Ganiyu</t>
+  </si>
+  <si>
+    <t>081112412380</t>
+  </si>
+  <si>
+    <t>0230173012901370</t>
+  </si>
+  <si>
+    <t>Dewi Dania</t>
+  </si>
+  <si>
+    <t>087592382939</t>
+  </si>
+  <si>
+    <t>1830183901839201</t>
+  </si>
+  <si>
+    <t>Zara Ghufran</t>
+  </si>
+  <si>
+    <t>083809813087</t>
+  </si>
+  <si>
+    <t>6219829182378910</t>
+  </si>
+  <si>
+    <t>086571892173</t>
+  </si>
+  <si>
+    <t>Anissa Van Hemmer</t>
+  </si>
+  <si>
+    <t>7287387381901821</t>
+  </si>
+  <si>
+    <t>Toto Harmono</t>
+  </si>
+  <si>
+    <t>087632832998</t>
+  </si>
+  <si>
+    <t>9212982901384802</t>
+  </si>
+  <si>
+    <t>Attiya Ana Valensi</t>
+  </si>
+  <si>
+    <t>086632942308</t>
+  </si>
+  <si>
+    <t>8218373899010101</t>
+  </si>
+  <si>
+    <t>Yudi Mahabrata</t>
+  </si>
+  <si>
+    <t>081520193812</t>
+  </si>
+  <si>
+    <t>5286137126829003</t>
+  </si>
+  <si>
+    <t>087821028390</t>
+  </si>
+  <si>
+    <t>Tivon Otegi</t>
+  </si>
+  <si>
+    <t>6423874832732829</t>
+  </si>
+  <si>
+    <t>Hansel Tanaka Permana</t>
+  </si>
+  <si>
+    <t>085629318910</t>
+  </si>
+  <si>
+    <t>2893718927138100</t>
+  </si>
+  <si>
+    <t>Vina Aquila Avanti</t>
+  </si>
+  <si>
+    <t>087597134234</t>
+  </si>
+  <si>
+    <t>Shahabi Hilman Rain</t>
+  </si>
+  <si>
+    <t>085621982387</t>
+  </si>
+  <si>
+    <t>4324783924793969</t>
+  </si>
+  <si>
+    <t>5589723874832422</t>
+  </si>
+  <si>
+    <t>Kevin Agila Frianto</t>
+  </si>
+  <si>
+    <t>083213821083</t>
+  </si>
+  <si>
+    <t>3892018392010101</t>
+  </si>
+  <si>
+    <t>Karina Albar Vashti</t>
+  </si>
+  <si>
+    <t>085521381281</t>
+  </si>
+  <si>
+    <t>3218371917391912</t>
+  </si>
+  <si>
+    <t>Jessica Galicia</t>
+  </si>
+  <si>
+    <t>081366667778</t>
+  </si>
+  <si>
+    <t>9283902839021001</t>
+  </si>
+  <si>
+    <t>Tevin Aura Arditi</t>
+  </si>
+  <si>
+    <t>087129182389</t>
+  </si>
+  <si>
+    <t>7313891155555555</t>
+  </si>
+  <si>
+    <t>Mirza Pratiwi Arkanda</t>
+  </si>
+  <si>
+    <t>085772671997</t>
+  </si>
+  <si>
+    <t>PENGAWAS</t>
   </si>
 </sst>
 </file>
@@ -864,7 +1080,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -891,6 +1107,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1433,7 +1655,7 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1729,7 +1951,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1779,18 +2001,19 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,10 +2043,10 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>160</v>
+        <v>258</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
@@ -1832,28 +2055,207 @@
         <v>2007</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C6" s="1">
         <v>3</v>
       </c>
-      <c r="F4" s="11">
-        <v>39179.375</v>
-      </c>
+      <c r="D6" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="1">
+        <v>2007</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C8" s="1">
+        <v>2</v>
+      </c>
+      <c r="D8" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1</v>
+      </c>
+      <c r="D10" s="1">
+        <v>2007</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C11" s="1">
+        <v>2</v>
+      </c>
+      <c r="D11" s="1">
+        <v>2008</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3</v>
+      </c>
+      <c r="D12" s="1">
+        <v>2009</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F14" s="9"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F15" s="9"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F16" s="9"/>
+    </row>
+    <row r="17" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F17" s="9"/>
+    </row>
+    <row r="18" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F18" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37" customWidth="1"/>
     <col min="3" max="3" width="4.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1862,6 +2264,11 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>276</v>
+      </c>
+    </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>158</v>
@@ -1875,14 +2282,276 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C4" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C4" s="1">
-        <v>1</v>
-      </c>
+      <c r="B5" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C5" s="13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="C7" s="13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C8" s="13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C9" s="13">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C10" s="13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C11" s="13">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C12" s="13">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>269</v>
+      </c>
+      <c r="C13" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C14" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C15" s="1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C16" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="C17" s="1">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C18" s="1">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" s="1">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C20" s="1">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C21" s="1">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1891,19 +2560,19 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.42578125" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" customWidth="1"/>
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="12.28515625" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="30.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -1911,44 +2580,389 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>328</v>
+      </c>
+    </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>164</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>165</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="7" t="s">
         <v>168</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>169</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D4" s="7" t="s">
         <v>160</v>
       </c>
-      <c r="F4" s="1">
+      <c r="E4" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F4" s="7">
         <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D5" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="F5" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E7" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="F7" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>297</v>
+      </c>
+      <c r="D11" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="F11" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>298</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>299</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="D12" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>303</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="F13" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="D14" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>315</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>160</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>317</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>321</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>270</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>327</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -2378,8 +3392,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H49" sqref="H49"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2439,10 +3453,10 @@
         <v>2</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>10</v>
@@ -2462,10 +3476,10 @@
         <v>2</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>11</v>
@@ -2485,10 +3499,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>12</v>
@@ -2505,10 +3519,10 @@
         <v>2</v>
       </c>
       <c r="F7" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="G7" s="7" t="s">
         <v>170</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>171</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>13</v>
@@ -2525,10 +3539,10 @@
         <v>2</v>
       </c>
       <c r="F8" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="G8" s="7" t="s">
         <v>172</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>173</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>14</v>
@@ -2545,10 +3559,10 @@
         <v>3</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>10</v>
@@ -2565,10 +3579,10 @@
         <v>3</v>
       </c>
       <c r="F10" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="G10" s="7" t="s">
         <v>200</v>
-      </c>
-      <c r="G10" s="7" t="s">
-        <v>201</v>
       </c>
       <c r="H10" s="1" t="s">
         <v>11</v>
@@ -2585,10 +3599,10 @@
         <v>3</v>
       </c>
       <c r="F11" s="7" t="s">
+        <v>201</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>202</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>203</v>
       </c>
       <c r="H11" s="1" t="s">
         <v>12</v>
@@ -2605,10 +3619,10 @@
         <v>3</v>
       </c>
       <c r="F12" s="7" t="s">
+        <v>173</v>
+      </c>
+      <c r="G12" s="7" t="s">
         <v>174</v>
-      </c>
-      <c r="G12" s="7" t="s">
-        <v>175</v>
       </c>
       <c r="H12" s="1" t="s">
         <v>13</v>
@@ -2625,10 +3639,10 @@
         <v>3</v>
       </c>
       <c r="F13" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="G13" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="H13" s="1" t="s">
         <v>14</v>
@@ -2645,10 +3659,10 @@
         <v>4</v>
       </c>
       <c r="F14" s="7" t="s">
+        <v>205</v>
+      </c>
+      <c r="G14" s="7" t="s">
         <v>206</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>207</v>
       </c>
       <c r="H14" s="1" t="s">
         <v>10</v>
@@ -2665,10 +3679,10 @@
         <v>4</v>
       </c>
       <c r="F15" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G15" s="7" t="s">
         <v>208</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>209</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>11</v>
@@ -2685,10 +3699,10 @@
         <v>4</v>
       </c>
       <c r="F16" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="G16" s="7" t="s">
         <v>210</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>211</v>
       </c>
       <c r="H16" s="1" t="s">
         <v>12</v>
@@ -2705,10 +3719,10 @@
         <v>4</v>
       </c>
       <c r="F17" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="7" t="s">
         <v>212</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>213</v>
       </c>
       <c r="H17" s="1" t="s">
         <v>13</v>
@@ -2725,10 +3739,10 @@
         <v>4</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G18" s="7" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="H18" s="1" t="s">
         <v>14</v>
@@ -2745,10 +3759,10 @@
         <v>2</v>
       </c>
       <c r="F19" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="G19" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="G19" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="H19" s="1" t="s">
         <v>10</v>
@@ -2765,10 +3779,10 @@
         <v>2</v>
       </c>
       <c r="F20" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="G20" s="7" t="s">
         <v>217</v>
-      </c>
-      <c r="G20" s="7" t="s">
-        <v>218</v>
       </c>
       <c r="H20" s="1" t="s">
         <v>11</v>
@@ -2785,10 +3799,10 @@
         <v>2</v>
       </c>
       <c r="F21" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="G21" s="7" t="s">
         <v>219</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>220</v>
       </c>
       <c r="H21" s="1" t="s">
         <v>12</v>
@@ -2805,10 +3819,10 @@
         <v>2</v>
       </c>
       <c r="F22" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="G22" s="7" t="s">
         <v>178</v>
-      </c>
-      <c r="G22" s="7" t="s">
-        <v>179</v>
       </c>
       <c r="H22" s="1" t="s">
         <v>13</v>
@@ -2825,10 +3839,10 @@
         <v>2</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G23" s="7" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H23" s="1" t="s">
         <v>14</v>
@@ -2845,10 +3859,10 @@
         <v>3</v>
       </c>
       <c r="F24" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="G24" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="H24" s="1" t="s">
         <v>10</v>
@@ -2865,10 +3879,10 @@
         <v>3</v>
       </c>
       <c r="F25" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="G25" s="7" t="s">
         <v>223</v>
-      </c>
-      <c r="G25" s="7" t="s">
-        <v>224</v>
       </c>
       <c r="H25" s="1" t="s">
         <v>11</v>
@@ -2885,10 +3899,10 @@
         <v>3</v>
       </c>
       <c r="F26" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="G26" s="7" t="s">
         <v>225</v>
-      </c>
-      <c r="G26" s="7" t="s">
-        <v>226</v>
       </c>
       <c r="H26" s="1" t="s">
         <v>12</v>
@@ -2905,10 +3919,10 @@
         <v>3</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>13</v>
@@ -2925,10 +3939,10 @@
         <v>3</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="G28" s="7" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="H28" s="1" t="s">
         <v>14</v>
@@ -2945,10 +3959,10 @@
         <v>4</v>
       </c>
       <c r="F29" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="G29" s="7" t="s">
         <v>227</v>
-      </c>
-      <c r="G29" s="7" t="s">
-        <v>228</v>
       </c>
       <c r="H29" s="1" t="s">
         <v>10</v>
@@ -2965,10 +3979,10 @@
         <v>4</v>
       </c>
       <c r="F30" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="G30" s="7" t="s">
         <v>229</v>
-      </c>
-      <c r="G30" s="7" t="s">
-        <v>230</v>
       </c>
       <c r="H30" s="1" t="s">
         <v>11</v>
@@ -2985,10 +3999,10 @@
         <v>4</v>
       </c>
       <c r="F31" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="G31" s="7" t="s">
         <v>231</v>
-      </c>
-      <c r="G31" s="7" t="s">
-        <v>232</v>
       </c>
       <c r="H31" s="1" t="s">
         <v>12</v>
@@ -3005,10 +4019,10 @@
         <v>4</v>
       </c>
       <c r="F32" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="G32" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="G32" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="H32" s="1" t="s">
         <v>13</v>
@@ -3025,10 +4039,10 @@
         <v>4</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>14</v>
@@ -3045,10 +4059,10 @@
         <v>2</v>
       </c>
       <c r="F34" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="G34" s="7" t="s">
         <v>236</v>
-      </c>
-      <c r="G34" s="7" t="s">
-        <v>237</v>
       </c>
       <c r="H34" s="1" t="s">
         <v>10</v>
@@ -3065,10 +4079,10 @@
         <v>2</v>
       </c>
       <c r="F35" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="G35" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="H35" s="1" t="s">
         <v>11</v>
@@ -3085,10 +4099,10 @@
         <v>2</v>
       </c>
       <c r="F36" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="G36" s="7" t="s">
         <v>240</v>
-      </c>
-      <c r="G36" s="7" t="s">
-        <v>241</v>
       </c>
       <c r="H36" s="1" t="s">
         <v>12</v>
@@ -3105,10 +4119,10 @@
         <v>2</v>
       </c>
       <c r="F37" s="7" t="s">
+        <v>185</v>
+      </c>
+      <c r="G37" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="G37" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="H37" s="1" t="s">
         <v>13</v>
@@ -3125,10 +4139,10 @@
         <v>2</v>
       </c>
       <c r="F38" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="G38" s="7" t="s">
         <v>188</v>
-      </c>
-      <c r="G38" s="7" t="s">
-        <v>189</v>
       </c>
       <c r="H38" s="1" t="s">
         <v>14</v>
@@ -3145,10 +4159,10 @@
         <v>3</v>
       </c>
       <c r="F39" s="7" t="s">
+        <v>241</v>
+      </c>
+      <c r="G39" s="7" t="s">
         <v>242</v>
-      </c>
-      <c r="G39" s="7" t="s">
-        <v>243</v>
       </c>
       <c r="H39" s="1" t="s">
         <v>10</v>
@@ -3165,10 +4179,10 @@
         <v>3</v>
       </c>
       <c r="F40" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="G40" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="G40" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="H40" s="1" t="s">
         <v>11</v>
@@ -3185,10 +4199,10 @@
         <v>3</v>
       </c>
       <c r="F41" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="G41" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="H41" s="1" t="s">
         <v>12</v>
@@ -3205,10 +4219,10 @@
         <v>3</v>
       </c>
       <c r="F42" s="7" t="s">
+        <v>189</v>
+      </c>
+      <c r="G42" s="7" t="s">
         <v>190</v>
-      </c>
-      <c r="G42" s="7" t="s">
-        <v>191</v>
       </c>
       <c r="H42" s="1" t="s">
         <v>13</v>
@@ -3225,10 +4239,10 @@
         <v>3</v>
       </c>
       <c r="F43" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="G43" s="7" t="s">
         <v>192</v>
-      </c>
-      <c r="G43" s="7" t="s">
-        <v>193</v>
       </c>
       <c r="H43" s="1" t="s">
         <v>14</v>
@@ -3245,10 +4259,10 @@
         <v>4</v>
       </c>
       <c r="F44" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G44" s="7" t="s">
         <v>248</v>
-      </c>
-      <c r="G44" s="7" t="s">
-        <v>249</v>
       </c>
       <c r="H44" s="1" t="s">
         <v>10</v>
@@ -3265,10 +4279,10 @@
         <v>4</v>
       </c>
       <c r="F45" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="G45" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="G45" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="H45" s="1" t="s">
         <v>11</v>
@@ -3285,10 +4299,10 @@
         <v>4</v>
       </c>
       <c r="F46" s="7" t="s">
+        <v>251</v>
+      </c>
+      <c r="G46" s="7" t="s">
         <v>252</v>
-      </c>
-      <c r="G46" s="7" t="s">
-        <v>253</v>
       </c>
       <c r="H46" s="1" t="s">
         <v>12</v>
@@ -3305,10 +4319,10 @@
         <v>4</v>
       </c>
       <c r="F47" s="7" t="s">
+        <v>253</v>
+      </c>
+      <c r="G47" s="7" t="s">
         <v>254</v>
-      </c>
-      <c r="G47" s="7" t="s">
-        <v>255</v>
       </c>
       <c r="H47" s="1" t="s">
         <v>13</v>
@@ -3325,10 +4339,10 @@
         <v>4</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G48" s="7" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="H48" s="1" t="s">
         <v>14</v>

</xml_diff>

<commit_message>
commit trigger/stored procedure a
</commit_message>
<xml_diff>
--- a/Data SIRIMA Mod B16.xlsx
+++ b/Data SIRIMA Mod B16.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="4635" firstSheet="15" activeTab="16"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="4635" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="JENJANG" sheetId="1" r:id="rId1"/>
@@ -2562,8 +2562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2975,7 +2975,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4626,8 +4626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G5"/>
   <sheetViews>
-    <sheetView topLeftCell="C2" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4700,8 +4700,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I4"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:I4"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>